<commit_message>
working on replacing coprodB with WEO data
</commit_message>
<xml_diff>
--- a/project_open_entrance/01_external_data/WEO/data/data_template.xlsx
+++ b/project_open_entrance/01_external_data/WEO/data/data_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\beukeladvd\Documents\GitHub\tno-eco-mod-ci\project_open_entrance\01_external_data\WEO\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{672BA101-DC45-4540-B02A-F9F24C4D29AC}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B21498B-2BD1-4889-AFE8-DE0F9D6C4A4B}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="340" yWindow="340" windowWidth="6970" windowHeight="7270" xr2:uid="{C65CA019-535F-433C-8C6B-8F79F595CBB3}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{C65CA019-535F-433C-8C6B-8F79F595CBB3}"/>
   </bookViews>
   <sheets>
     <sheet name="Electricity" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="836" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="837" uniqueCount="130">
   <si>
     <t>Coal</t>
   </si>
@@ -790,7 +790,7 @@
   <dimension ref="A2:AR362"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1581,7 +1581,9 @@
       <c r="A8" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="1"/>
+      <c r="B8" s="1" t="s">
+        <v>4</v>
+      </c>
       <c r="C8" s="1">
         <v>290</v>
       </c>

</xml_diff>